<commit_message>
added economy of scale to network generation
</commit_message>
<xml_diff>
--- a/Assignment1_Problem1_Datasheets_v2.xlsx
+++ b/Assignment1_Problem1_Datasheets_v2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blopesdossanto\surfdrive\01 TU Delft\02 Education\02 Courses\2021_2022\AE4423-Airline Planning &amp; Optimization\Assignment AE4423\2021_2022\Assignment Part 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fab16832d8cf965b/Repositories/AE4423-Airline_Planning_and_Optimisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_1432B53CBE0BAB30A0D5E4B9EAD5AD93C97798B3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="19" activeTab="30"/>
+    <workbookView xWindow="-25200" yWindow="330" windowWidth="18900" windowHeight="11055" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="72" r:id="rId1"/>
@@ -566,7 +567,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -950,7 +951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1220,7 +1221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2285,11 +2286,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3080,7 +3081,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -3873,7 +3874,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4652,7 +4653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5712,7 +5713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6507,7 +6508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7318,7 +7319,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8098,7 +8099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9162,7 +9163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9955,7 +9956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11135,7 +11136,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11941,7 +11942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -12719,7 +12720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13781,7 +13782,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -14573,7 +14574,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15378,7 +15379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -16157,7 +16158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17219,7 +17220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -18013,7 +18014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18819,7 +18820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19597,7 +19598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20385,7 +20386,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21446,10 +21447,10 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -22251,7 +22252,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23057,7 +23058,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -23835,7 +23836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24900,7 +24901,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -25679,7 +25680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26507,7 +26508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -27285,6 +27286,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA7A90D6A9C6744D851BC705B70AE9DE" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed565d9e59d99895393132493f298f40">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3edf358e-6b25-4c9c-b2f8-9ff413806a29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="807c1b201ae6d81ab7b0cfd660fa2c9e" ns2:_="">
     <xsd:import namespace="3edf358e-6b25-4c9c-b2f8-9ff413806a29"/>
@@ -27462,22 +27478,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1B71822-2A1B-4E6B-B467-D552F8700615}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9968BD6A-E5D3-4B0B-AF00-22968D5578FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0958A4D2-0EE3-42BD-983F-4CB810A71711}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27493,21 +27511,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9968BD6A-E5D3-4B0B-AF00-22968D5578FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1B71822-2A1B-4E6B-B467-D552F8700615}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>